<commit_message>
example excel doc tweak
</commit_message>
<xml_diff>
--- a/example_excel_files/Example Excel Template.xlsx
+++ b/example_excel_files/Example Excel Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TooFastDan\Documents\MD_PhD Application\Cycle Analyzer\example_excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0B8D59-DCE6-421F-8DED-B6C561A86678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446DA379-DB0E-4A70-90AA-4BE12B3369A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{0F127685-172B-4FDA-90F6-58D0273CA525}"/>
+    <workbookView xWindow="-28920" yWindow="6075" windowWidth="29040" windowHeight="16440" xr2:uid="{0F127685-172B-4FDA-90F6-58D0273CA525}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -214,7 +214,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8599C06-C79F-4017-B909-83140B8550C5}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +544,7 @@
     <col min="5" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -570,7 +570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -583,11 +583,8 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -605,12 +602,11 @@
         <v>44571</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -622,12 +618,11 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -639,12 +634,11 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -658,12 +652,11 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -677,9 +670,11 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -693,7 +688,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -713,7 +708,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -733,7 +728,7 @@
         <v>44553</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -751,7 +746,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -765,7 +760,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -779,7 +774,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -795,7 +790,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -815,7 +810,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>

</xml_diff>